<commit_message>
replaced all files in repo; new versions are updated are exactly the same as the previous version -KL
</commit_message>
<xml_diff>
--- a/August 2013 waypoints raw.xlsx
+++ b/August 2013 waypoints raw.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="459">
   <si>
     <t>type</t>
   </si>
@@ -1390,6 +1390,9 @@
   </si>
   <si>
     <t>t_gps</t>
+  </si>
+  <si>
+    <t>likely an inaccurate gps point due to proximety</t>
   </si>
 </sst>
 </file>
@@ -1737,10 +1740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J419"/>
+  <dimension ref="A1:K419"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z37" sqref="Z33:AC37"/>
+    <sheetView tabSelected="1" topLeftCell="E145" workbookViewId="0">
+      <selection activeCell="L155" sqref="L155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6264,7 +6267,7 @@
         <v>41491.646643518521</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>456</v>
       </c>
@@ -6296,7 +6299,7 @@
         <v>41491.648414351854</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>456</v>
       </c>
@@ -6328,7 +6331,7 @@
         <v>41491.630312499998</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>456</v>
       </c>
@@ -6360,7 +6363,7 @@
         <v>41491.63318287037</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>456</v>
       </c>
@@ -6392,7 +6395,7 @@
         <v>41486.342002314814</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>456</v>
       </c>
@@ -6424,7 +6427,7 @@
         <v>41494.71266203704</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>456</v>
       </c>
@@ -6454,7 +6457,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>456</v>
       </c>
@@ -6486,7 +6489,7 @@
         <v>41486.754618055558</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>456</v>
       </c>
@@ -6518,7 +6521,7 @@
         <v>41488.465578703705</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>456</v>
       </c>
@@ -6549,8 +6552,11 @@
       <c r="J153" s="2">
         <v>41486.707291666666</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K153" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>456</v>
       </c>
@@ -6582,7 +6588,7 @@
         <v>41490.463842592595</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>456</v>
       </c>
@@ -6614,7 +6620,7 @@
         <v>41496.403101851851</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>456</v>
       </c>
@@ -6646,7 +6652,7 @@
         <v>41488.536736111113</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>456</v>
       </c>
@@ -6678,7 +6684,7 @@
         <v>41490.414525462962</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>456</v>
       </c>
@@ -6710,7 +6716,7 @@
         <v>41489.515462962961</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>456</v>
       </c>
@@ -6742,7 +6748,7 @@
         <v>41496.390300925923</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>456</v>
       </c>

</xml_diff>